<commit_message>
Creación de Excel con datos de evaluaciones
</commit_message>
<xml_diff>
--- a/data/Datos Evaluación.xlsx
+++ b/data/Datos Evaluación.xlsx
@@ -8,45 +8,46 @@
   </bookViews>
   <sheets>
     <sheet name="Evaluación 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Evaluación 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
   <si>
     <t>Fecha</t>
   </si>
   <si>
-    <t>Pregunta1</t>
-  </si>
-  <si>
-    <t>Pregunta2</t>
-  </si>
-  <si>
-    <t>Pregunta3</t>
-  </si>
-  <si>
-    <t>Pregunta4</t>
-  </si>
-  <si>
-    <t>Pregunta5</t>
-  </si>
-  <si>
-    <t>Pregunta6</t>
-  </si>
-  <si>
-    <t>Pregunta7</t>
-  </si>
-  <si>
-    <t>Pregunta8</t>
-  </si>
-  <si>
-    <t>Pregunta9</t>
-  </si>
-  <si>
-    <t>Pregunta10</t>
+    <t>Gerencia</t>
+  </si>
+  <si>
+    <t>Cédula</t>
+  </si>
+  <si>
+    <t>Nombre Líder</t>
+  </si>
+  <si>
+    <t>Nombre Practicante</t>
+  </si>
+  <si>
+    <t>Pregunta 1</t>
+  </si>
+  <si>
+    <t>Pregunta 2</t>
+  </si>
+  <si>
+    <t>Pregunta 3</t>
+  </si>
+  <si>
+    <t>Pregunta 4</t>
+  </si>
+  <si>
+    <t>Pregunta 5</t>
+  </si>
+  <si>
+    <t>Pregunta 6</t>
   </si>
   <si>
     <t>Observaciones</t>
@@ -128,6 +129,45 @@
   </si>
   <si>
     <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>2022-12-14</t>
+  </si>
+  <si>
+    <t>M&amp;O</t>
+  </si>
+  <si>
+    <t>Ejemploooooo oooooooo ooooooooooooooo</t>
+  </si>
+  <si>
+    <t>13240</t>
+  </si>
+  <si>
+    <t>10000001231</t>
+  </si>
+  <si>
+    <t>Javier Sarmiento</t>
+  </si>
+  <si>
+    <t>Ejemploooooooooo oooooooooo ooooooooo</t>
+  </si>
+  <si>
+    <t>Julian Cely</t>
+  </si>
+  <si>
+    <t>Ejemplooooooo ooo oooooo ooooooooooooo</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Que hambre</t>
+  </si>
+  <si>
+    <t>Aquí va una observación</t>
   </si>
 </sst>
 </file>
@@ -186,8 +226,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -490,157 +533,312 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creación de archivos excel desde la app
</commit_message>
<xml_diff>
--- a/data/Datos Evaluación.xlsx
+++ b/data/Datos Evaluación.xlsx
@@ -226,11 +226,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -534,169 +531,169 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>29</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -713,131 +710,131 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>48</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flechas para retornar a home
</commit_message>
<xml_diff>
--- a/data/Datos Evaluación.xlsx
+++ b/data/Datos Evaluación.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
   <si>
     <t>Fecha</t>
   </si>
@@ -56,7 +56,7 @@
     <t>2022-11-16</t>
   </si>
   <si>
-    <t>2022-11-04</t>
+    <t>2023-01-18</t>
   </si>
   <si>
     <t>2022-11-23</t>
@@ -65,7 +65,7 @@
     <t>pepito</t>
   </si>
   <si>
-    <t>dsfg</t>
+    <t>Mantenimiento Acceso</t>
   </si>
   <si>
     <t>Experiencia al cliente</t>
@@ -74,7 +74,7 @@
     <t>00000</t>
   </si>
   <si>
-    <t>12345dsfdf</t>
+    <t>1234567890</t>
   </si>
   <si>
     <t>123456789</t>
@@ -83,7 +83,7 @@
     <t>nn</t>
   </si>
   <si>
-    <t>cvcbv</t>
+    <t>Javier Sarmiento</t>
   </si>
   <si>
     <t>Ejemplo ejemplo</t>
@@ -92,7 +92,7 @@
     <t>andre</t>
   </si>
   <si>
-    <t>scvdf</t>
+    <t>Julián David Cely Forero</t>
   </si>
   <si>
     <t>Yesid Sanabria</t>
@@ -101,7 +101,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>5</t>
+    <t>10</t>
   </si>
   <si>
     <t>9</t>
@@ -110,61 +110,55 @@
     <t>2</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Flojo</t>
+  </si>
+  <si>
+    <t>Buen desempeño</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>2023-01-25</t>
+  </si>
+  <si>
+    <t>2022-12-14</t>
+  </si>
+  <si>
+    <t>asdfghj</t>
+  </si>
+  <si>
+    <t>Ejemploooooo oooooooo ooooooooooooooo</t>
+  </si>
+  <si>
+    <t>2345678</t>
+  </si>
+  <si>
+    <t>10000001231</t>
+  </si>
+  <si>
+    <t>sdfghjk</t>
+  </si>
+  <si>
+    <t>Ejemploooooooooo oooooooooo ooooooooo</t>
+  </si>
+  <si>
+    <t>fdgfhjh,</t>
+  </si>
+  <si>
+    <t>Ejemplooooooo ooo oooooo ooooooooooooo</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Flojo</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur.</t>
-  </si>
-  <si>
-    <t>Ejemplo</t>
-  </si>
-  <si>
-    <t>2022-12-14</t>
-  </si>
-  <si>
-    <t>M&amp;O</t>
-  </si>
-  <si>
-    <t>Ejemploooooo oooooooo ooooooooooooooo</t>
-  </si>
-  <si>
-    <t>13240</t>
-  </si>
-  <si>
-    <t>10000001231</t>
-  </si>
-  <si>
-    <t>Javier Sarmiento</t>
-  </si>
-  <si>
-    <t>Ejemploooooooooo oooooooooo ooooooooo</t>
-  </si>
-  <si>
-    <t>Julian Cely</t>
-  </si>
-  <si>
-    <t>Ejemplooooooo ooo oooooo ooooooooooooo</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Que hambre</t>
+    <t>asdfkyglh,nbmvxjfdtifyogluñj</t>
   </si>
   <si>
     <t>Aquí va una observación</t>
@@ -536,7 +530,12 @@
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="11" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -613,7 +612,7 @@
         <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -636,22 +635,22 @@
         <v>28</v>
       </c>
       <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -674,13 +673,13 @@
         <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
         <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
         <v>29</v>
@@ -689,7 +688,7 @@
         <v>29</v>
       </c>
       <c r="L4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -710,7 +709,12 @@
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="11" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -754,78 +758,78 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>47</v>
-      </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
         <v>46</v>
       </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>